<commit_message>
Added script to create sql tables for each player
</commit_message>
<xml_diff>
--- a/player_names.xlsx
+++ b/player_names.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="1362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="1407">
   <si>
     <t>MS Wade</t>
   </si>
@@ -1342,33 +1342,51 @@
     <t>Sharjeel Khan</t>
   </si>
   <si>
+    <t>Mohammad Rizwan</t>
+  </si>
+  <si>
+    <t>Imad Wasim</t>
+  </si>
+  <si>
+    <t>Mohammad Nawaz (3)</t>
+  </si>
+  <si>
     <t>Asad Shafiq</t>
   </si>
   <si>
-    <t>Imad Wasim</t>
-  </si>
-  <si>
-    <t>Mohammad Rizwan</t>
-  </si>
-  <si>
     <t>PSP Handscomb</t>
   </si>
   <si>
+    <t>Junaid Khan</t>
+  </si>
+  <si>
     <t>A Zampa</t>
   </si>
   <si>
+    <t>BJ Watling</t>
+  </si>
+  <si>
+    <t>C Munro</t>
+  </si>
+  <si>
+    <t>C de Grandhomme</t>
+  </si>
+  <si>
+    <t>LH Ferguson</t>
+  </si>
+  <si>
     <t>Noor Ali Zadran</t>
   </si>
   <si>
     <t>Mirwais Ashraf</t>
   </si>
   <si>
+    <t>MH Cross</t>
+  </si>
+  <si>
     <t>CD Wallace</t>
   </si>
   <si>
-    <t>MH Cross</t>
-  </si>
-  <si>
     <t>RD Berrington</t>
   </si>
   <si>
@@ -1378,9 +1396,45 @@
     <t>SM Sharif</t>
   </si>
   <si>
+    <t>RAJ Smith</t>
+  </si>
+  <si>
+    <t>AC Evans</t>
+  </si>
+  <si>
+    <t>BTJ Wheal</t>
+  </si>
+  <si>
+    <t>Nizakat Khan</t>
+  </si>
+  <si>
+    <t>Aizaz Khan</t>
+  </si>
+  <si>
+    <t>Ehsan Khan</t>
+  </si>
+  <si>
+    <t>Tanwir Afzal</t>
+  </si>
+  <si>
     <t>MRJ Watt</t>
   </si>
   <si>
+    <t>C Carter</t>
+  </si>
+  <si>
+    <t>Shahid Wasif</t>
+  </si>
+  <si>
+    <t>Waqas Khan</t>
+  </si>
+  <si>
+    <t>Nadeem Ahmed</t>
+  </si>
+  <si>
+    <t>Tanveer Ahmed</t>
+  </si>
+  <si>
     <t>PJ Moor</t>
   </si>
   <si>
@@ -1393,6 +1447,9 @@
     <t>T Muzarabani</t>
   </si>
   <si>
+    <t>KK Nair</t>
+  </si>
+  <si>
     <t>T Maruma</t>
   </si>
   <si>
@@ -1402,10 +1459,7 @@
     <t>T Mupariwa</t>
   </si>
   <si>
-    <t>C Munro</t>
-  </si>
-  <si>
-    <t>LH Ferguson</t>
+    <t>FY Fazal</t>
   </si>
   <si>
     <t>Sabbir Rahman</t>
@@ -1414,27 +1468,51 @@
     <t>Mosaddek Hossain</t>
   </si>
   <si>
+    <t>Taskin Ahmed</t>
+  </si>
+  <si>
+    <t>Tanbir Hayder</t>
+  </si>
+  <si>
     <t>Nurul Hasan</t>
   </si>
   <si>
-    <t>Tanbir Hayder</t>
-  </si>
-  <si>
-    <t>Taskin Ahmed</t>
+    <t>Subashis Roy</t>
+  </si>
+  <si>
+    <t>SD Heazlett</t>
   </si>
   <si>
     <t>DG Brownlie</t>
   </si>
   <si>
-    <t>C de Grandhomme</t>
-  </si>
-  <si>
     <t>AL Phehlukwayo</t>
   </si>
   <si>
     <t>AF Milne</t>
   </si>
   <si>
+    <t>MC Henriques</t>
+  </si>
+  <si>
+    <t>N Dickwella</t>
+  </si>
+  <si>
+    <t>DAS Gunaratne</t>
+  </si>
+  <si>
+    <t>S Prasanna</t>
+  </si>
+  <si>
+    <t>RAS Lakmal</t>
+  </si>
+  <si>
+    <t>N Pradeep</t>
+  </si>
+  <si>
+    <t>Shadab Khan</t>
+  </si>
+  <si>
     <t>Mehedi Hasan Miraz</t>
   </si>
   <si>
@@ -1444,45 +1522,12 @@
     <t>MA Wood</t>
   </si>
   <si>
-    <t>MC Henriques</t>
-  </si>
-  <si>
-    <t>N Dickwella</t>
-  </si>
-  <si>
-    <t>DAS Gunaratne</t>
-  </si>
-  <si>
-    <t>RAS Lakmal</t>
-  </si>
-  <si>
-    <t>N Pradeep</t>
-  </si>
-  <si>
-    <t>C Carter</t>
+    <t>Fahim Ashraf</t>
   </si>
   <si>
     <t>KD Shah</t>
   </si>
   <si>
-    <t>Nizakat Khan</t>
-  </si>
-  <si>
-    <t>Shahid Wasif</t>
-  </si>
-  <si>
-    <t>Ehsan Khan</t>
-  </si>
-  <si>
-    <t>Tanwir Afzal</t>
-  </si>
-  <si>
-    <t>Aizaz Khan</t>
-  </si>
-  <si>
-    <t>Nadeem Ahmed</t>
-  </si>
-  <si>
     <t>TP Ura</t>
   </si>
   <si>
@@ -1498,19 +1543,28 @@
     <t>S Bau</t>
   </si>
   <si>
+    <t>MD Dai</t>
+  </si>
+  <si>
     <t>D Bau</t>
   </si>
   <si>
-    <t>MD Dai</t>
-  </si>
-  <si>
     <t>H Hiri</t>
   </si>
   <si>
+    <t>N Vanua</t>
+  </si>
+  <si>
+    <t>WT Gavera</t>
+  </si>
+  <si>
     <t>JB Reva</t>
   </si>
   <si>
-    <t>N Vanua</t>
+    <t>JJ Atkinson</t>
+  </si>
+  <si>
+    <t>K Christie</t>
   </si>
   <si>
     <t>SW Billings</t>
@@ -1534,10 +1588,13 @@
     <t>AR Nurse</t>
   </si>
   <si>
+    <t>D Bishoo</t>
+  </si>
+  <si>
     <t>ST Gabriel</t>
   </si>
   <si>
-    <t>D Bishoo</t>
+    <t>AS Joseph</t>
   </si>
   <si>
     <t>A Balbirnie</t>
@@ -1555,24 +1612,33 @@
     <t>DJ Willey</t>
   </si>
   <si>
+    <t>BJ McCarthy</t>
+  </si>
+  <si>
     <t>JM Vince</t>
   </si>
   <si>
     <t>BM Duckett</t>
   </si>
   <si>
+    <t>Mosharraf Hossain</t>
+  </si>
+  <si>
     <t>DAJ Bracewell</t>
   </si>
   <si>
     <t>AP Devcich</t>
   </si>
   <si>
-    <t>BJ Watling</t>
-  </si>
-  <si>
     <t>AR Patel</t>
   </si>
   <si>
+    <t>UT Yadav</t>
+  </si>
+  <si>
+    <t>DS Kulkarni</t>
+  </si>
+  <si>
     <t>J Yadav</t>
   </si>
   <si>
@@ -1585,22 +1651,31 @@
     <t>SC Kuggeleijn</t>
   </si>
   <si>
-    <t>BJ McCarthy</t>
+    <t>Simi Singh</t>
+  </si>
+  <si>
+    <t>CA Young</t>
   </si>
   <si>
     <t>Hashmatullah Shahidi</t>
   </si>
   <si>
+    <t>J Mulder</t>
+  </si>
+  <si>
     <t>Shafiqullah</t>
   </si>
   <si>
     <t>Dawlat Zadran</t>
   </si>
   <si>
+    <t>AR McBrine</t>
+  </si>
+  <si>
     <t>Usman Ghani</t>
   </si>
   <si>
-    <t>AR McBrine</t>
+    <t>Najeeb Tarakai</t>
   </si>
   <si>
     <t>S Jafta</t>
@@ -1615,30 +1690,33 @@
     <t>Sharmin Akhter</t>
   </si>
   <si>
+    <t>Fargana Hoque</t>
+  </si>
+  <si>
+    <t>Rumana Ahmed</t>
+  </si>
+  <si>
+    <t>Nigar Sultana</t>
+  </si>
+  <si>
+    <t>Salma Khatun</t>
+  </si>
+  <si>
     <t>Shaila Sharmin</t>
   </si>
   <si>
-    <t>Rumana Ahmed</t>
-  </si>
-  <si>
-    <t>Nigar Sultana</t>
-  </si>
-  <si>
-    <t>Salma Khatun</t>
-  </si>
-  <si>
-    <t>Fargana Hoque</t>
+    <t>Nahida Akter</t>
+  </si>
+  <si>
+    <t>Khadija Tul Kubra</t>
+  </si>
+  <si>
+    <t>Panna Ghosh</t>
   </si>
   <si>
     <t>Lata Mondal</t>
   </si>
   <si>
-    <t>Panna Ghosh</t>
-  </si>
-  <si>
-    <t>Khadija Tul Kubra</t>
-  </si>
-  <si>
     <t>D Devnarain</t>
   </si>
   <si>
@@ -1648,15 +1726,27 @@
     <t>GM Harris</t>
   </si>
   <si>
+    <t>ML Schutt</t>
+  </si>
+  <si>
+    <t>KM Beams</t>
+  </si>
+  <si>
     <t>BL Mooney</t>
   </si>
   <si>
-    <t>ML Schutt</t>
-  </si>
-  <si>
     <t>A Wellington</t>
   </si>
   <si>
+    <t>L Goodall</t>
+  </si>
+  <si>
+    <t>A Bosch</t>
+  </si>
+  <si>
+    <t>M Daniels</t>
+  </si>
+  <si>
     <t>PM Weerakkody</t>
   </si>
   <si>
@@ -1681,7 +1771,13 @@
     <t>BMSM Kumari</t>
   </si>
   <si>
-    <t>Mohammad Nawaz (3)</t>
+    <t>GWHM Perera</t>
+  </si>
+  <si>
+    <t>KADA Kanchana</t>
+  </si>
+  <si>
+    <t>SJ Benn</t>
   </si>
   <si>
     <t>RH Priest</t>
@@ -1699,15 +1795,15 @@
     <t>Nahida Khan</t>
   </si>
   <si>
+    <t>Nain Abidi</t>
+  </si>
+  <si>
     <t>Bismah Maroof</t>
   </si>
   <si>
     <t>Nida Dar</t>
   </si>
   <si>
-    <t>Nain Abidi</t>
-  </si>
-  <si>
     <t>Asmavia Iqbal</t>
   </si>
   <si>
@@ -1726,6 +1822,9 @@
     <t>Sadia Yousuf</t>
   </si>
   <si>
+    <t>SRH Curtis</t>
+  </si>
+  <si>
     <t>RL Haynes</t>
   </si>
   <si>
@@ -1744,19 +1843,19 @@
     <t>EM Bermingham</t>
   </si>
   <si>
-    <t>SRH Curtis</t>
+    <t>A Gardner</t>
   </si>
   <si>
     <t>AC Kerr</t>
   </si>
   <si>
-    <t>Mosharraf Hossain</t>
-  </si>
-  <si>
-    <t>GWHM Perera</t>
-  </si>
-  <si>
-    <t>KADA Kanchana</t>
+    <t>Shabir Noori</t>
+  </si>
+  <si>
+    <t>Naveen-ul-Haq</t>
+  </si>
+  <si>
+    <t>Nawroz Mangal</t>
   </si>
   <si>
     <t>OU Ranasinghe</t>
@@ -1765,21 +1864,39 @@
     <t>SS Weerakkody</t>
   </si>
   <si>
+    <t>L Winfield</t>
+  </si>
+  <si>
+    <t>DN Wyatt</t>
+  </si>
+  <si>
+    <t>FC Wilson</t>
+  </si>
+  <si>
     <t>AE Jones</t>
   </si>
   <si>
-    <t>DN Wyatt</t>
-  </si>
-  <si>
-    <t>FC Wilson</t>
-  </si>
-  <si>
     <t>D Hazell</t>
   </si>
   <si>
     <t>BA Langston</t>
   </si>
   <si>
+    <t>HML Madushani</t>
+  </si>
+  <si>
+    <t>MAA Sanjeewani</t>
+  </si>
+  <si>
+    <t>H Karunaratne</t>
+  </si>
+  <si>
+    <t>NND de Silva</t>
+  </si>
+  <si>
+    <t>WGAKK Kulasuriya</t>
+  </si>
+  <si>
     <t>BB Chari</t>
   </si>
   <si>
@@ -1792,9 +1909,6 @@
     <t>R Powell</t>
   </si>
   <si>
-    <t>SJ Benn</t>
-  </si>
-  <si>
     <t>GSNFG Jayasuriya</t>
   </si>
   <si>
@@ -1804,21 +1918,78 @@
     <t>TK Musakanda</t>
   </si>
   <si>
-    <t>H Karunaratne</t>
-  </si>
-  <si>
     <t>A Nao</t>
   </si>
   <si>
+    <t>Rohan Mustafa</t>
+  </si>
+  <si>
+    <t>Mohammed Qasim</t>
+  </si>
+  <si>
+    <t>Ghulam Shabber</t>
+  </si>
+  <si>
+    <t>Shaiman Anwar</t>
+  </si>
+  <si>
+    <t>Muhammad Usman</t>
+  </si>
+  <si>
+    <t>Rameez Shahzad</t>
+  </si>
+  <si>
+    <t>Mohammad Naveed</t>
+  </si>
+  <si>
+    <t>Ahmed Raza</t>
+  </si>
+  <si>
+    <t>Zahoor Khan</t>
+  </si>
+  <si>
     <t>H Kaur</t>
   </si>
   <si>
     <t>V Krishnamurthy</t>
   </si>
   <si>
+    <t>M Shehani</t>
+  </si>
+  <si>
     <t>Rabiya Shah</t>
   </si>
   <si>
+    <t>MV Waldron</t>
+  </si>
+  <si>
+    <t>CNIM Joyce</t>
+  </si>
+  <si>
+    <t>KJ Garth</t>
+  </si>
+  <si>
+    <t>L Delany</t>
+  </si>
+  <si>
+    <t>IMHC Joyce</t>
+  </si>
+  <si>
+    <t>GH Lewis</t>
+  </si>
+  <si>
+    <t>CMA Shillington</t>
+  </si>
+  <si>
+    <t>RA Lewis</t>
+  </si>
+  <si>
+    <t>LN McCarthy</t>
+  </si>
+  <si>
+    <t>CJ Metcalfe</t>
+  </si>
+  <si>
     <t>Aiman Anwer</t>
   </si>
   <si>
@@ -1828,52 +1999,34 @@
     <t>Sanjida Islam</t>
   </si>
   <si>
+    <t>SM Kavanagh</t>
+  </si>
+  <si>
+    <t>AJ Kenealy</t>
+  </si>
+  <si>
     <t>Suraiya Azmin</t>
   </si>
   <si>
     <t>S Verma</t>
   </si>
   <si>
+    <t>Y Fourie</t>
+  </si>
+  <si>
+    <t>MM Letsoalo</t>
+  </si>
+  <si>
     <t>MF Kendal</t>
   </si>
   <si>
-    <t>CNIM Joyce</t>
-  </si>
-  <si>
-    <t>KJ Garth</t>
-  </si>
-  <si>
-    <t>CMA Shillington</t>
-  </si>
-  <si>
-    <t>L Delany</t>
-  </si>
-  <si>
-    <t>IMHC Joyce</t>
-  </si>
-  <si>
-    <t>GH Lewis</t>
-  </si>
-  <si>
-    <t>MV Waldron</t>
-  </si>
-  <si>
-    <t>RA Lewis</t>
-  </si>
-  <si>
     <t>LK O'Reilly</t>
   </si>
   <si>
-    <t>CJ Metcalfe</t>
-  </si>
-  <si>
     <t>Maham Tariq</t>
   </si>
   <si>
-    <t>AJ Kenealy</t>
-  </si>
-  <si>
-    <t>MM Letsoalo</t>
+    <t>Poonam Yadav</t>
   </si>
   <si>
     <t>CAK Walton</t>
@@ -1888,78 +2041,45 @@
     <t>CB Sole</t>
   </si>
   <si>
-    <t>BTJ Wheal</t>
-  </si>
-  <si>
     <t>C McAuslan</t>
   </si>
   <si>
-    <t>Waqas Khan</t>
-  </si>
-  <si>
     <t>Ehsan Nawaz</t>
   </si>
   <si>
-    <t>Tanveer Ahmed</t>
-  </si>
-  <si>
     <t>RP Burl</t>
   </si>
   <si>
     <t>R Ngarava</t>
   </si>
   <si>
+    <t>Fareed Ahmad</t>
+  </si>
+  <si>
     <t>Ihsanullah</t>
   </si>
   <si>
     <t>Karim Janat</t>
   </si>
   <si>
-    <t>Fareed Ahmad</t>
-  </si>
-  <si>
-    <t>CA Young</t>
-  </si>
-  <si>
-    <t>Rohan Mustafa</t>
-  </si>
-  <si>
-    <t>Mohammad Naveed</t>
-  </si>
-  <si>
-    <t>Ghulam Shabber</t>
-  </si>
-  <si>
-    <t>Shaiman Anwar</t>
-  </si>
-  <si>
-    <t>Rameez Shahzad</t>
-  </si>
-  <si>
-    <t>Muhammad Usman</t>
-  </si>
-  <si>
-    <t>Ahmed Raza</t>
-  </si>
-  <si>
     <t>Amjad Javed</t>
   </si>
   <si>
-    <t>Zahoor Khan</t>
-  </si>
-  <si>
     <t>TAM Siriwardana</t>
   </si>
   <si>
+    <t>CBRLS Kumara</t>
+  </si>
+  <si>
     <t>MDK Perera</t>
   </si>
   <si>
-    <t>S Prasanna</t>
-  </si>
-  <si>
     <t>HASD Siriwardene</t>
   </si>
   <si>
+    <t>A Hartley</t>
+  </si>
+  <si>
     <t>Kainat Imtiaz</t>
   </si>
   <si>
@@ -1999,54 +2119,33 @@
     <t>M Joshi</t>
   </si>
   <si>
-    <t>Poonam Yadav</t>
-  </si>
-  <si>
     <t>R Boyce</t>
   </si>
   <si>
     <t>Q Joseph</t>
   </si>
   <si>
-    <t>L Winfield</t>
-  </si>
-  <si>
-    <t>A Gardner</t>
-  </si>
-  <si>
     <t>SE Aley</t>
   </si>
   <si>
+    <t>Marina Iqbal</t>
+  </si>
+  <si>
     <t>Kycia A Knight</t>
   </si>
   <si>
     <t>AK Peters</t>
   </si>
   <si>
-    <t>Marina Iqbal</t>
-  </si>
-  <si>
-    <t>M Daniels</t>
-  </si>
-  <si>
-    <t>A Hartley</t>
-  </si>
-  <si>
-    <t>KM Beams</t>
-  </si>
-  <si>
-    <t>Mohammed Qasim</t>
-  </si>
-  <si>
-    <t>AC Evans</t>
+    <t>ML Green</t>
+  </si>
+  <si>
+    <t>JNT Vare</t>
   </si>
   <si>
     <t>L Paul</t>
   </si>
   <si>
-    <t>SM Kavanagh</t>
-  </si>
-  <si>
     <t>J Gray</t>
   </si>
   <si>
@@ -2068,21 +2167,33 @@
     <t>R Ntozakhe</t>
   </si>
   <si>
+    <t>R Stokell</t>
+  </si>
+  <si>
+    <t>L Little</t>
+  </si>
+  <si>
+    <t>RS Gayakwad</t>
+  </si>
+  <si>
     <t>Afsar Zazai</t>
   </si>
   <si>
+    <t>RL Chase</t>
+  </si>
+  <si>
+    <t>ML Cummins</t>
+  </si>
+  <si>
     <t>KA Hope</t>
   </si>
   <si>
-    <t>RL Chase</t>
-  </si>
-  <si>
-    <t>AS Joseph</t>
-  </si>
-  <si>
     <t>KOK Williams</t>
   </si>
   <si>
+    <t>Kuldeep Yadav</t>
+  </si>
+  <si>
     <t>LD Madushanka</t>
   </si>
   <si>
@@ -2104,6 +2215,30 @@
     <t>G Chapple</t>
   </si>
   <si>
+    <t>DI Joyce</t>
+  </si>
+  <si>
+    <t>AC Botha</t>
+  </si>
+  <si>
+    <t>WK McCallan</t>
+  </si>
+  <si>
+    <t>PG Gillespie</t>
+  </si>
+  <si>
+    <t>AR White</t>
+  </si>
+  <si>
+    <t>D Langford-Smith</t>
+  </si>
+  <si>
+    <t>JF Mooney</t>
+  </si>
+  <si>
+    <t>PJK Mooney</t>
+  </si>
+  <si>
     <t>R Clarke</t>
   </si>
   <si>
@@ -2122,13 +2257,22 @@
     <t>Iftikhar Anjum</t>
   </si>
   <si>
+    <t>MH Yardy</t>
+  </si>
+  <si>
     <t>RP Arnold</t>
   </si>
   <si>
+    <t>TT Bresnan</t>
+  </si>
+  <si>
+    <t>SJ Harmison</t>
+  </si>
+  <si>
     <t>VS Solanki</t>
   </si>
   <si>
-    <t>TT Bresnan</t>
+    <t>Kabir Ali</t>
   </si>
   <si>
     <t>SM Katich</t>
@@ -2137,24 +2281,36 @@
     <t>SR Clark</t>
   </si>
   <si>
+    <t>AG Prince</t>
+  </si>
+  <si>
     <t>PA Jaques</t>
   </si>
   <si>
     <t>BR Dorey</t>
   </si>
   <si>
+    <t>JJ van der Wath</t>
+  </si>
+  <si>
+    <t>J Botha</t>
+  </si>
+  <si>
+    <t>GJP Kruger</t>
+  </si>
+  <si>
+    <t>JA Rudolph</t>
+  </si>
+  <si>
     <t>MS Atapattu</t>
   </si>
   <si>
+    <t>GB Hogg</t>
+  </si>
+  <si>
     <t>WCA Ganegama</t>
   </si>
   <si>
-    <t>JJ van der Wath</t>
-  </si>
-  <si>
-    <t>JA Rudolph</t>
-  </si>
-  <si>
     <t>DA Gunawardene</t>
   </si>
   <si>
@@ -2176,6 +2332,18 @@
     <t>Mohammad Sami</t>
   </si>
   <si>
+    <t>D Ganga</t>
+  </si>
+  <si>
+    <t>WW Hinds</t>
+  </si>
+  <si>
+    <t>RN Lewis</t>
+  </si>
+  <si>
+    <t>IDR Bradshaw</t>
+  </si>
+  <si>
     <t>Rajin Saleh</t>
   </si>
   <si>
@@ -2200,30 +2368,27 @@
     <t>KHRK Fernando</t>
   </si>
   <si>
+    <t>Javed Omar</t>
+  </si>
+  <si>
     <t>KS Lokuarachchi</t>
   </si>
   <si>
+    <t>Manjural Islam Rana</t>
+  </si>
+  <si>
     <t>Tushar Imran</t>
   </si>
   <si>
     <t>Shahadat Hossain</t>
   </si>
   <si>
-    <t>D Ganga</t>
-  </si>
-  <si>
-    <t>WW Hinds</t>
-  </si>
-  <si>
-    <t>IDR Bradshaw</t>
+    <t>DK Butler</t>
   </si>
   <si>
     <t>ID Blackwell</t>
   </si>
   <si>
-    <t>Kabir Ali</t>
-  </si>
-  <si>
     <t>RR Powar</t>
   </si>
   <si>
@@ -2233,7 +2398,7 @@
     <t>VRV Singh</t>
   </si>
   <si>
-    <t>GB Hogg</t>
+    <t>RV Uthappa</t>
   </si>
   <si>
     <t>RJ Peterson</t>
@@ -2242,6 +2407,9 @@
     <t>R Telemachus</t>
   </si>
   <si>
+    <t>ML Lewis</t>
+  </si>
+  <si>
     <t>KTGD Prasad</t>
   </si>
   <si>
@@ -2272,28 +2440,97 @@
     <t>AJ Ireland</t>
   </si>
   <si>
+    <t>S Chattergoon</t>
+  </si>
+  <si>
     <t>CS Baugh</t>
   </si>
   <si>
-    <t>S Chattergoon</t>
-  </si>
-  <si>
-    <t>RV Uthappa</t>
+    <t>KO Meth</t>
   </si>
   <si>
     <t>CD Collymore</t>
   </si>
   <si>
-    <t>AC Botha</t>
-  </si>
-  <si>
-    <t>AR White</t>
-  </si>
-  <si>
-    <t>WK McCallan</t>
-  </si>
-  <si>
-    <t>D Langford-Smith</t>
+    <t>DF Watts</t>
+  </si>
+  <si>
+    <t>NS Poonia</t>
+  </si>
+  <si>
+    <t>RR Watson</t>
+  </si>
+  <si>
+    <t>GM Hamilton</t>
+  </si>
+  <si>
+    <t>DR Brown</t>
+  </si>
+  <si>
+    <t>CJO Smith</t>
+  </si>
+  <si>
+    <t>CM Wright</t>
+  </si>
+  <si>
+    <t>GA Rogers</t>
+  </si>
+  <si>
+    <t>CJ Smith</t>
+  </si>
+  <si>
+    <t>OL Pitcher</t>
+  </si>
+  <si>
+    <t>DL Hemp</t>
+  </si>
+  <si>
+    <t>IH Romaine</t>
+  </si>
+  <si>
+    <t>JJ Tucker</t>
+  </si>
+  <si>
+    <t>DA Minors</t>
+  </si>
+  <si>
+    <t>LOB Cann</t>
+  </si>
+  <si>
+    <t>DCC Borden</t>
+  </si>
+  <si>
+    <t>KAD Hurdle</t>
+  </si>
+  <si>
+    <t>RDM Leverock</t>
+  </si>
+  <si>
+    <t>S Matsikenyeri</t>
+  </si>
+  <si>
+    <t>B Zuiderent</t>
+  </si>
+  <si>
+    <t>DJ Reekers</t>
+  </si>
+  <si>
+    <t>AN Kervezee</t>
+  </si>
+  <si>
+    <t>DLS van Bunge</t>
+  </si>
+  <si>
+    <t>ES Szwarczynski</t>
+  </si>
+  <si>
+    <t>TBM de Leede</t>
+  </si>
+  <si>
+    <t>PW Borren</t>
+  </si>
+  <si>
+    <t>LP van Troost</t>
   </si>
   <si>
     <t>MP Vaughan</t>
@@ -2305,121 +2542,100 @@
     <t>Azhar Mahmood</t>
   </si>
   <si>
+    <t>J Smits</t>
+  </si>
+  <si>
+    <t>Adeel Raja</t>
+  </si>
+  <si>
+    <t>MBS Jonkman</t>
+  </si>
+  <si>
+    <t>GEF Barnett</t>
+  </si>
+  <si>
+    <t>IS Billcliff</t>
+  </si>
+  <si>
+    <t>AM Samad</t>
+  </si>
+  <si>
+    <t>AA Mulla</t>
+  </si>
+  <si>
+    <t>DR Chumney</t>
+  </si>
+  <si>
+    <t>SD Outerbridge</t>
+  </si>
+  <si>
+    <t>MO Jones</t>
+  </si>
+  <si>
     <t>F Kasteni</t>
   </si>
   <si>
-    <t>S Matsikenyeri</t>
-  </si>
-  <si>
-    <t>DF Watts</t>
-  </si>
-  <si>
-    <t>RR Watson</t>
-  </si>
-  <si>
-    <t>GM Hamilton</t>
-  </si>
-  <si>
     <t>NFI McCallum</t>
   </si>
   <si>
-    <t>DR Brown</t>
-  </si>
-  <si>
-    <t>CJO Smith</t>
-  </si>
-  <si>
     <t>JAR Blain</t>
   </si>
   <si>
     <t>PJC Hoffmann</t>
   </si>
   <si>
+    <t>MA Ouma</t>
+  </si>
+  <si>
+    <t>DO Obuya</t>
+  </si>
+  <si>
+    <t>RD Shah</t>
+  </si>
+  <si>
+    <t>SO Tikolo</t>
+  </si>
+  <si>
+    <t>JK Kamande</t>
+  </si>
+  <si>
+    <t>LN Onyango</t>
+  </si>
+  <si>
+    <t>PJ Ongondo</t>
+  </si>
+  <si>
+    <t>HA Varaiya</t>
+  </si>
+  <si>
     <t>Danish Kaneria</t>
   </si>
   <si>
-    <t>NS Poonia</t>
-  </si>
-  <si>
-    <t>CM Wright</t>
-  </si>
-  <si>
-    <t>GA Rogers</t>
-  </si>
-  <si>
-    <t>JF Mooney</t>
-  </si>
-  <si>
-    <t>MA Ouma</t>
-  </si>
-  <si>
-    <t>RD Shah</t>
+    <t>U Bhatti</t>
+  </si>
+  <si>
+    <t>AC Cummins</t>
+  </si>
+  <si>
+    <t>KT Sandher</t>
   </si>
   <si>
     <t>AO Suji</t>
   </si>
   <si>
-    <t>SO Tikolo</t>
-  </si>
-  <si>
-    <t>JK Kamande</t>
-  </si>
-  <si>
-    <t>LN Onyango</t>
-  </si>
-  <si>
-    <t>PJ Ongondo</t>
-  </si>
-  <si>
-    <t>HA Varaiya</t>
-  </si>
-  <si>
-    <t>SD Outerbridge</t>
-  </si>
-  <si>
-    <t>OL Pitcher</t>
-  </si>
-  <si>
-    <t>DCC Borden</t>
-  </si>
-  <si>
-    <t>DL Hemp</t>
-  </si>
-  <si>
-    <t>IH Romaine</t>
-  </si>
-  <si>
-    <t>DA Minors</t>
-  </si>
-  <si>
-    <t>LOB Cann</t>
-  </si>
-  <si>
-    <t>JJ Tucker</t>
-  </si>
-  <si>
-    <t>KAD Hurdle</t>
-  </si>
-  <si>
-    <t>Javed Omar</t>
-  </si>
-  <si>
-    <t>PJK Mooney</t>
+    <t>WB Rankin</t>
   </si>
   <si>
     <t>MS Panesar</t>
   </si>
   <si>
-    <t>WB Rankin</t>
-  </si>
-  <si>
-    <t>AG Prince</t>
+    <t>DS Smith</t>
   </si>
   <si>
     <t>KED Carroll</t>
   </si>
   <si>
-    <t>DS Smith</t>
+    <t>MR Gillespie</t>
   </si>
   <si>
     <t>TV Mufambisi</t>
@@ -2428,18 +2644,18 @@
     <t>LE Bosman</t>
   </si>
   <si>
+    <t>W Jaffer</t>
+  </si>
+  <si>
+    <t>D Mongia</t>
+  </si>
+  <si>
+    <t>A Kumble</t>
+  </si>
+  <si>
     <t>VVS Laxman</t>
   </si>
   <si>
-    <t>D Mongia</t>
-  </si>
-  <si>
-    <t>A Kumble</t>
-  </si>
-  <si>
-    <t>MR Gillespie</t>
-  </si>
-  <si>
     <t>MB Loye</t>
   </si>
   <si>
@@ -2455,6 +2671,9 @@
     <t>NN Odhiambo</t>
   </si>
   <si>
+    <t>Farhad Reza</t>
+  </si>
+  <si>
     <t>JS Ababu</t>
   </si>
   <si>
@@ -2467,15 +2686,6 @@
     <t>T Kamungozi</t>
   </si>
   <si>
-    <t>Farhad Reza</t>
-  </si>
-  <si>
-    <t>MH Yardy</t>
-  </si>
-  <si>
-    <t>SJ Harmison</t>
-  </si>
-  <si>
     <t>Abdur Rehman</t>
   </si>
   <si>
@@ -2485,6 +2695,9 @@
     <t>AR Adams</t>
   </si>
   <si>
+    <t>DR Tuffey</t>
+  </si>
+  <si>
     <t>AN Petersen</t>
   </si>
   <si>
@@ -2500,6 +2713,9 @@
     <t>AD Mascarenhas</t>
   </si>
   <si>
+    <t>RJ Sidebottom</t>
+  </si>
+  <si>
     <t>PP Chawla</t>
   </si>
   <si>
@@ -2512,64 +2728,31 @@
     <t>RD Steede</t>
   </si>
   <si>
-    <t>RDM Leverock</t>
-  </si>
-  <si>
-    <t>B Zuiderent</t>
-  </si>
-  <si>
-    <t>ES Szwarczynski</t>
-  </si>
-  <si>
-    <t>DLS van Bunge</t>
-  </si>
-  <si>
-    <t>AN Kervezee</t>
-  </si>
-  <si>
-    <t>TBM de Leede</t>
-  </si>
-  <si>
-    <t>PW Borren</t>
-  </si>
-  <si>
-    <t>LP van Troost</t>
-  </si>
-  <si>
-    <t>J Smits</t>
-  </si>
-  <si>
-    <t>MBS Jonkman</t>
+    <t>DES Maxwell</t>
   </si>
   <si>
     <t>Mohammad Kashif</t>
   </si>
   <si>
-    <t>CJ Smith</t>
-  </si>
-  <si>
     <t>H Durham</t>
   </si>
   <si>
     <t>SKW Kelly</t>
   </si>
   <si>
-    <t>AA Mulla</t>
-  </si>
-  <si>
-    <t>AM Samad</t>
-  </si>
-  <si>
-    <t>DR Chumney</t>
+    <t>S Jyoti</t>
   </si>
   <si>
     <t>Qaiser Ali</t>
   </si>
   <si>
-    <t>DES Maxwell</t>
-  </si>
-  <si>
-    <t>U Bhatti</t>
+    <t>S Thuraisingam</t>
+  </si>
+  <si>
+    <t>TN de Grooth</t>
+  </si>
+  <si>
+    <t>MWA van Nierop</t>
   </si>
   <si>
     <t>Mehrab Hossain jnr</t>
@@ -2581,36 +2764,30 @@
     <t>ML Nkala</t>
   </si>
   <si>
-    <t>AC Cummins</t>
-  </si>
-  <si>
-    <t>MO Jones</t>
-  </si>
-  <si>
     <t>ADJ Pitcher</t>
   </si>
   <si>
     <t>RT Lyons</t>
   </si>
   <si>
-    <t>DO Obuya</t>
+    <t>A Codrington</t>
+  </si>
+  <si>
+    <t>RR Emrit</t>
   </si>
   <si>
     <t>P Mustard</t>
   </si>
   <si>
-    <t>RJ Sidebottom</t>
-  </si>
-  <si>
     <t>MS Sinclair</t>
   </si>
   <si>
+    <t>GJ Hopkins</t>
+  </si>
+  <si>
     <t>MKDI Amerasinghe</t>
   </si>
   <si>
-    <t>DI Joyce</t>
-  </si>
-  <si>
     <t>MJ Fourie</t>
   </si>
   <si>
@@ -2650,30 +2827,27 @@
     <t>D Soraine</t>
   </si>
   <si>
+    <t>AA Obanda</t>
+  </si>
+  <si>
     <t>TR Ambrose</t>
   </si>
   <si>
     <t>DR Flynn</t>
   </si>
   <si>
-    <t>GJ Hopkins</t>
-  </si>
-  <si>
-    <t>J Botha</t>
-  </si>
-  <si>
     <t>Fawad Alam</t>
   </si>
   <si>
     <t>BA Parchment</t>
   </si>
   <si>
+    <t>JL Ontong</t>
+  </si>
+  <si>
     <t>PA Browne</t>
   </si>
   <si>
-    <t>RN Lewis</t>
-  </si>
-  <si>
     <t>Junaid Siddique</t>
   </si>
   <si>
@@ -2704,6 +2878,9 @@
     <t>KC Hodsoll</t>
   </si>
   <si>
+    <t>AS Luseno</t>
+  </si>
+  <si>
     <t>RW Price</t>
   </si>
   <si>
@@ -2722,6 +2899,12 @@
     <t>ADS Fletcher</t>
   </si>
   <si>
+    <t>SE Findlay</t>
+  </si>
+  <si>
+    <t>NO Miller</t>
+  </si>
+  <si>
     <t>Raqibul Hasan</t>
   </si>
   <si>
@@ -2740,13 +2923,10 @@
     <t>GH O'Brien</t>
   </si>
   <si>
-    <t>AA Obanda</t>
-  </si>
-  <si>
-    <t>DJ Reekers</t>
-  </si>
-  <si>
-    <t>TN de Grooth</t>
+    <t>HS Baidwan</t>
+  </si>
+  <si>
+    <t>Sami Faridi</t>
   </si>
   <si>
     <t>HJC Mol</t>
@@ -2773,9 +2953,84 @@
     <t>C Zhuwao</t>
   </si>
   <si>
+    <t>PC Connell</t>
+  </si>
+  <si>
     <t>Kamran Hussain</t>
   </si>
   <si>
+    <t>Khalid Latif</t>
+  </si>
+  <si>
+    <t>Khurram Manzoor</t>
+  </si>
+  <si>
+    <t>Arshad Ali</t>
+  </si>
+  <si>
+    <t>IPP Batuwitarachchi</t>
+  </si>
+  <si>
+    <t>Saqib Ali</t>
+  </si>
+  <si>
+    <t>V Shetty</t>
+  </si>
+  <si>
+    <t>Mohammad Tauqir</t>
+  </si>
+  <si>
+    <t>EHSN Silva</t>
+  </si>
+  <si>
+    <t>Zahid Shah</t>
+  </si>
+  <si>
+    <t>Fahad Alhashmi</t>
+  </si>
+  <si>
+    <t>Tabarak Dar</t>
+  </si>
+  <si>
+    <t>Skhawat Ali</t>
+  </si>
+  <si>
+    <t>KH Butt</t>
+  </si>
+  <si>
+    <t>Irfan Ahmed</t>
+  </si>
+  <si>
+    <t>CK Kruger</t>
+  </si>
+  <si>
+    <t>Zain Abbas</t>
+  </si>
+  <si>
+    <t>Munir Dar</t>
+  </si>
+  <si>
+    <t>Najeeb Amar</t>
+  </si>
+  <si>
+    <t>JPR Lamsam</t>
+  </si>
+  <si>
+    <t>Afzaal Haider</t>
+  </si>
+  <si>
+    <t>N Fernandes</t>
+  </si>
+  <si>
+    <t>Alawi Shukri</t>
+  </si>
+  <si>
+    <t>Aman Ali</t>
+  </si>
+  <si>
+    <t>Mansoor Amjad</t>
+  </si>
+  <si>
     <t>PP Ojha</t>
   </si>
   <si>
@@ -2797,9 +3052,6 @@
     <t>PM Siddle</t>
   </si>
   <si>
-    <t>JL Ontong</t>
-  </si>
-  <si>
     <t>J Louw</t>
   </si>
   <si>
@@ -2809,21 +3061,30 @@
     <t>RE van der Merwe</t>
   </si>
   <si>
+    <t>B Geeves</t>
+  </si>
+  <si>
+    <t>SM Harwood</t>
+  </si>
+  <si>
     <t>ND McKenzie</t>
   </si>
   <si>
     <t>VB van Jaarsveld</t>
   </si>
   <si>
+    <t>IE O'Brien</t>
+  </si>
+  <si>
     <t>CD Cumming</t>
   </si>
   <si>
+    <t>BJ Diamanti</t>
+  </si>
+  <si>
     <t>GJ Batty</t>
   </si>
   <si>
-    <t>NO Miller</t>
-  </si>
-  <si>
     <t>LS Baker</t>
   </si>
   <si>
@@ -2845,24 +3106,36 @@
     <t>G Sultana</t>
   </si>
   <si>
+    <t>SC Taylor</t>
+  </si>
+  <si>
+    <t>SR Waters</t>
+  </si>
+  <si>
+    <t>IG Butler</t>
+  </si>
+  <si>
     <t>PD McGlashan</t>
   </si>
   <si>
     <t>BP Nash</t>
   </si>
   <si>
-    <t>SE Findlay</t>
-  </si>
-  <si>
-    <t>Khurram Manzoor</t>
-  </si>
-  <si>
     <t>Saeed Ajmal</t>
   </si>
   <si>
     <t>SHT Kandamby</t>
   </si>
   <si>
+    <t>DE Bernard</t>
+  </si>
+  <si>
+    <t>Mahbubul Alam</t>
+  </si>
+  <si>
+    <t>RM West</t>
+  </si>
+  <si>
     <t>S Nitschke</t>
   </si>
   <si>
@@ -2884,15 +3157,21 @@
     <t>SJ Andrews</t>
   </si>
   <si>
-    <t>SR Waters</t>
-  </si>
-  <si>
     <t>RR Patel</t>
   </si>
   <si>
     <t>RL Bhudia</t>
   </si>
   <si>
+    <t>F Mutizwa</t>
+  </si>
+  <si>
+    <t>Sohail Khan</t>
+  </si>
+  <si>
+    <t>L Balaji</t>
+  </si>
+  <si>
     <t>R McLaren</t>
   </si>
   <si>
@@ -2902,24 +3181,12 @@
     <t>JH Stander</t>
   </si>
   <si>
-    <t>GEF Barnett</t>
-  </si>
-  <si>
     <t>Rizwan Cheema</t>
   </si>
   <si>
-    <t>IS Billcliff</t>
-  </si>
-  <si>
-    <t>S Jyoti</t>
-  </si>
-  <si>
     <t>Karim Sadiq</t>
   </si>
   <si>
-    <t>Nawroz Mangal</t>
-  </si>
-  <si>
     <t>Raees Ahmadzai</t>
   </si>
   <si>
@@ -2938,13 +3205,13 @@
     <t>DM Richards</t>
   </si>
   <si>
+    <t>FL Reifer</t>
+  </si>
+  <si>
     <t>TM Dowlin</t>
   </si>
   <si>
-    <t>FL Reifer</t>
-  </si>
-  <si>
-    <t>DE Bernard</t>
+    <t>NT Pascal</t>
   </si>
   <si>
     <t>DC Thomas</t>
@@ -2953,27 +3220,24 @@
     <t>GC Tonge</t>
   </si>
   <si>
-    <t>IG Butler</t>
-  </si>
-  <si>
-    <t>Khalid Latif</t>
-  </si>
-  <si>
     <t>MA Vermeulen</t>
   </si>
   <si>
     <t>Enamul Haque jnr</t>
   </si>
   <si>
+    <t>H Patel</t>
+  </si>
+  <si>
     <t>TL Best</t>
   </si>
   <si>
-    <t>DR Tuffey</t>
-  </si>
-  <si>
     <t>RT Crandon</t>
   </si>
   <si>
+    <t>AM Nayar</t>
+  </si>
+  <si>
     <t>G Onions</t>
   </si>
   <si>
@@ -2986,9 +3250,6 @@
     <t>KM Jarvis</t>
   </si>
   <si>
-    <t>F Mutizwa</t>
-  </si>
-  <si>
     <t>PY Lavine</t>
   </si>
   <si>
@@ -3004,6 +3265,12 @@
     <t>SA Campbelle</t>
   </si>
   <si>
+    <t>K Thomson</t>
+  </si>
+  <si>
+    <t>SA Fritz</t>
+  </si>
+  <si>
     <t>PJ Ingram</t>
   </si>
   <si>
@@ -3019,6 +3286,9 @@
     <t>Jahurul Islam</t>
   </si>
   <si>
+    <t>A Shahzad</t>
+  </si>
+  <si>
     <t>UWMBCA Welegedara</t>
   </si>
   <si>
@@ -3028,16 +3298,40 @@
     <t>SO Ngoche</t>
   </si>
   <si>
+    <t>ZE Surkari</t>
+  </si>
+  <si>
+    <t>AS Hansra</t>
+  </si>
+  <si>
+    <t>TG Gordon</t>
+  </si>
+  <si>
+    <t>WD Balaji Rao</t>
+  </si>
+  <si>
+    <t>RW Chakabva</t>
+  </si>
+  <si>
     <t>W Barresi</t>
   </si>
   <si>
     <t>TLW Cooper</t>
   </si>
   <si>
+    <t>HMRKB Herath</t>
+  </si>
+  <si>
+    <t>BP Loots</t>
+  </si>
+  <si>
+    <t>BA Westdijk</t>
+  </si>
+  <si>
     <t>GA Lamb</t>
   </si>
   <si>
-    <t>RW Chakabva</t>
+    <t>NR Kumar</t>
   </si>
   <si>
     <t>JO Ngoche</t>
@@ -3046,48 +3340,39 @@
     <t>BP Kruger</t>
   </si>
   <si>
-    <t>A Shahzad</t>
-  </si>
-  <si>
     <t>AF Buurman</t>
   </si>
   <si>
-    <t>Adeel Raja</t>
-  </si>
-  <si>
-    <t>H Patel</t>
-  </si>
-  <si>
-    <t>ZE Surkari</t>
-  </si>
-  <si>
-    <t>AS Hansra</t>
-  </si>
-  <si>
-    <t>NR Kumar</t>
-  </si>
-  <si>
     <t>K Whatham</t>
   </si>
   <si>
-    <t>HS Baidwan</t>
-  </si>
-  <si>
-    <t>WD Balaji Rao</t>
-  </si>
-  <si>
     <t>JJ Krejza</t>
   </si>
   <si>
+    <t>KA Edwards</t>
+  </si>
+  <si>
     <t>LJ Woodcock</t>
   </si>
   <si>
     <t>AB Barath</t>
   </si>
   <si>
+    <t>A Mithun</t>
+  </si>
+  <si>
+    <t>S Tyagi</t>
+  </si>
+  <si>
     <t>PA Desai</t>
   </si>
   <si>
+    <t>AD Poynter</t>
+  </si>
+  <si>
+    <t>RD McCann</t>
+  </si>
+  <si>
     <t>DR Lockhart</t>
   </si>
   <si>
@@ -3100,27 +3385,27 @@
     <t>Shapoor Zadran</t>
   </si>
   <si>
+    <t>R Flannigan</t>
+  </si>
+  <si>
     <t>AM Blignaut</t>
   </si>
   <si>
     <t>AB Dinda</t>
   </si>
   <si>
-    <t>UT Yadav</t>
-  </si>
-  <si>
     <t>NV Ojha</t>
   </si>
   <si>
     <t>Pankaj Singh</t>
   </si>
   <si>
+    <t>Shahzaib Hasan</t>
+  </si>
+  <si>
     <t>Umar Amin</t>
   </si>
   <si>
-    <t>Shahzaib Hasan</t>
-  </si>
-  <si>
     <t>Zulqarnain Haider</t>
   </si>
   <si>
@@ -3130,37 +3415,34 @@
     <t>SW Masakadza</t>
   </si>
   <si>
+    <t>IA Nicolson</t>
+  </si>
+  <si>
+    <t>PA Patel</t>
+  </si>
+  <si>
+    <t>SS Tiwary</t>
+  </si>
+  <si>
     <t>TJ Heggelman</t>
   </si>
   <si>
     <t>MMA Jonkman</t>
   </si>
   <si>
-    <t>BP Loots</t>
-  </si>
-  <si>
-    <t>AD Poynter</t>
-  </si>
-  <si>
-    <t>RD McCann</t>
-  </si>
-  <si>
     <t>NG Jones</t>
   </si>
   <si>
     <t>A van der Merwe</t>
   </si>
   <si>
-    <t>HMRKB Herath</t>
-  </si>
-  <si>
     <t>WP Saha</t>
   </si>
   <si>
     <t>JW Dernbach</t>
   </si>
   <si>
-    <t>PA Patel</t>
+    <t>FDM Karunaratne</t>
   </si>
   <si>
     <t>R Vinay Kumar</t>
@@ -3169,27 +3451,18 @@
     <t>SG Borthwick</t>
   </si>
   <si>
-    <t>KO Meth</t>
-  </si>
-  <si>
-    <t>KA Edwards</t>
-  </si>
-  <si>
     <t>Hammad Azam</t>
   </si>
   <si>
+    <t>Mohammad Salman</t>
+  </si>
+  <si>
     <t>Usman Salahuddin</t>
   </si>
   <si>
-    <t>Mohammad Salman</t>
-  </si>
-  <si>
     <t>Tanvir Ahmed (1)</t>
   </si>
   <si>
-    <t>Junaid Khan</t>
-  </si>
-  <si>
     <t>Taufeeq Umar</t>
   </si>
   <si>
@@ -3205,6 +3478,9 @@
     <t>N Kruger</t>
   </si>
   <si>
+    <t>GI Maiden</t>
+  </si>
+  <si>
     <t>CKB Kulasekara</t>
   </si>
   <si>
@@ -3217,6 +3493,9 @@
     <t>DT Christian</t>
   </si>
   <si>
+    <t>R Sharma</t>
+  </si>
+  <si>
     <t>PJ Forrest</t>
   </si>
   <si>
@@ -3238,12 +3517,24 @@
     <t>Adnan Akmal</t>
   </si>
   <si>
+    <t>Usman Limbada</t>
+  </si>
+  <si>
+    <t>Hamza Tariq</t>
+  </si>
+  <si>
+    <t>Junaid Siddiqui</t>
+  </si>
+  <si>
+    <t>Zahid Hussain</t>
+  </si>
+  <si>
+    <t>N M'shangwe</t>
+  </si>
+  <si>
     <t>A Brindle</t>
   </si>
   <si>
-    <t>SA Fritz</t>
-  </si>
-  <si>
     <t>AL Hodgkinson</t>
   </si>
   <si>
@@ -3256,6 +3547,12 @@
     <t>D Elgar</t>
   </si>
   <si>
+    <t>VR Aaron</t>
+  </si>
+  <si>
+    <t>Elias Sunny</t>
+  </si>
+  <si>
     <t>S Naik</t>
   </si>
   <si>
@@ -3268,25 +3565,40 @@
     <t>R Malhotra</t>
   </si>
   <si>
+    <t>DI Allan</t>
+  </si>
+  <si>
+    <t>RG Aga</t>
+  </si>
+  <si>
     <t>Zakiullah Zaki</t>
   </si>
   <si>
     <t>Izatullah Dawlatzai</t>
   </si>
   <si>
+    <t>SJ Myburgh</t>
+  </si>
+  <si>
+    <t>MJ McClenaghan</t>
+  </si>
+  <si>
     <t>MC Sorensen</t>
   </si>
   <si>
     <t>MA Carberry</t>
   </si>
   <si>
+    <t>GS Ballance</t>
+  </si>
+  <si>
     <t>Fawad Ahmed</t>
   </si>
   <si>
     <t>RK Kleinveldt</t>
   </si>
   <si>
-    <t>MJ McClenaghan</t>
+    <t>AM Phangiso</t>
   </si>
   <si>
     <t>HD Rutherford</t>
@@ -3301,73 +3613,106 @@
     <t>SA Millanta</t>
   </si>
   <si>
+    <t>LR Doolan</t>
+  </si>
+  <si>
+    <t>SJ McGlashan</t>
+  </si>
+  <si>
     <t>FL Mackay</t>
   </si>
   <si>
-    <t>SJ McGlashan</t>
-  </si>
-  <si>
     <t>NJ Browne</t>
   </si>
   <si>
+    <t>RH Candy</t>
+  </si>
+  <si>
+    <t>SEA Ruck</t>
+  </si>
+  <si>
     <t>Mominul Haque</t>
   </si>
   <si>
     <t>Raza-ur-Rehman</t>
   </si>
   <si>
-    <t>Usman Limbada</t>
-  </si>
-  <si>
-    <t>Hamza Tariq</t>
+    <t>HL Colvin</t>
+  </si>
+  <si>
+    <t>HL Ferling</t>
   </si>
   <si>
     <t>CT Mutombodzi</t>
   </si>
   <si>
-    <t>N M'shangwe</t>
-  </si>
-  <si>
-    <t>HL Colvin</t>
+    <t>SL Quintyne</t>
+  </si>
+  <si>
+    <t>TD Smartt</t>
   </si>
   <si>
     <t>BYA Mendis</t>
   </si>
   <si>
+    <t>SK Dolawatte</t>
+  </si>
+  <si>
     <t>CR Seneviratna</t>
   </si>
   <si>
+    <t>KV Jain</t>
+  </si>
+  <si>
+    <t>S Sharma</t>
+  </si>
+  <si>
     <t>JL Hunter</t>
   </si>
   <si>
-    <t>HL Ferling</t>
-  </si>
-  <si>
-    <t>SK Dolawatte</t>
-  </si>
-  <si>
     <t>NY McLean</t>
   </si>
   <si>
-    <t>TD Smartt</t>
-  </si>
-  <si>
-    <t>LR Doolan</t>
+    <t>KE Broadmore</t>
+  </si>
+  <si>
+    <t>MJG Nielsen</t>
+  </si>
+  <si>
+    <t>LHD Dilhara</t>
   </si>
   <si>
     <t>Ehsan Adil</t>
   </si>
   <si>
+    <t>NM Carter</t>
+  </si>
+  <si>
+    <t>MW Machan</t>
+  </si>
+  <si>
+    <t>D Murphy</t>
+  </si>
+  <si>
+    <t>I Wardlaw</t>
+  </si>
+  <si>
+    <t>RML Taylor</t>
+  </si>
+  <si>
     <t>JNK Shannon</t>
   </si>
   <si>
     <t>Abul Hasan</t>
   </si>
   <si>
+    <t>JB Nero</t>
+  </si>
+  <si>
     <t>JW Ogle-Thomas</t>
   </si>
   <si>
-    <t>JB Nero</t>
+    <t>HAM Samuddika</t>
   </si>
   <si>
     <t>Robiul Islam</t>
@@ -3376,7 +3721,16 @@
     <t>Batool Fatima</t>
   </si>
   <si>
-    <t>GS Ballance</t>
+    <t>Qanita Jalil</t>
+  </si>
+  <si>
+    <t>Sumaiya Siddiqi</t>
+  </si>
+  <si>
+    <t>Ahsan Malik</t>
+  </si>
+  <si>
+    <t>AK Perera</t>
   </si>
   <si>
     <t>MJ Lumb</t>
@@ -3385,10 +3739,22 @@
     <t>MT Chinouya</t>
   </si>
   <si>
+    <t>CA Pujara</t>
+  </si>
+  <si>
     <t>Javeria Rauf</t>
   </si>
   <si>
-    <t>Qanita Jalil</t>
+    <t>MEMO Scott-Hayward</t>
+  </si>
+  <si>
+    <t>RA Rolfe</t>
+  </si>
+  <si>
+    <t>EJ Tice</t>
+  </si>
+  <si>
+    <t>EAJ Richardson</t>
   </si>
   <si>
     <t>Asad Ali</t>
@@ -3400,13 +3766,7 @@
     <t>HJW Gardiner</t>
   </si>
   <si>
-    <t>MW Machan</t>
-  </si>
-  <si>
-    <t>RML Taylor</t>
-  </si>
-  <si>
-    <t>I Wardlaw</t>
+    <t>Aftab Alam</t>
   </si>
   <si>
     <t>AR Berenger</t>
@@ -3418,27 +3778,27 @@
     <t>SP Patil</t>
   </si>
   <si>
-    <t>Mohammad Tauqir</t>
+    <t>FRJ Coleman</t>
   </si>
   <si>
     <t>AM Guruge</t>
   </si>
   <si>
-    <t>Sohail Khan</t>
-  </si>
-  <si>
     <t>Rahat Ali</t>
   </si>
   <si>
     <t>Arafat Sunny</t>
   </si>
   <si>
+    <t>Saqlain Haider</t>
+  </si>
+  <si>
+    <t>Kamran Shazad</t>
+  </si>
+  <si>
     <t>Nasir Jamal</t>
   </si>
   <si>
-    <t>FRJ Coleman</t>
-  </si>
-  <si>
     <t>Nasir Aziz</t>
   </si>
   <si>
@@ -3454,28 +3814,19 @@
     <t>KDK Vithanage</t>
   </si>
   <si>
-    <t>SJ Myburgh</t>
-  </si>
-  <si>
     <t>BN Cooper</t>
   </si>
   <si>
-    <t>Ahsan Malik</t>
-  </si>
-  <si>
     <t>D Daesrath</t>
   </si>
   <si>
-    <t>Junaid Siddiqui</t>
-  </si>
-  <si>
     <t>K Kamyuka</t>
   </si>
   <si>
     <t>JOA Gordon</t>
   </si>
   <si>
-    <t>D Murphy</t>
+    <t>EJ Richardson</t>
   </si>
   <si>
     <t>Ayasha Rahman</t>
@@ -3487,6 +3838,9 @@
     <t>Ritu Moni</t>
   </si>
   <si>
+    <t>A le Breton</t>
+  </si>
+  <si>
     <t>Shathira Jakir</t>
   </si>
   <si>
@@ -3496,51 +3850,48 @@
     <t>Sultana Yesmin</t>
   </si>
   <si>
+    <t>KL Cross</t>
+  </si>
+  <si>
     <t>HF Gurney</t>
   </si>
   <si>
-    <t>HAM Samuddika</t>
-  </si>
-  <si>
     <t>SDNS Karunaratne</t>
   </si>
   <si>
     <t>RS Vandort</t>
   </si>
   <si>
-    <t>FDM Karunaratne</t>
-  </si>
-  <si>
-    <t>RG Aga</t>
+    <t>Al-Amin Hossain</t>
+  </si>
+  <si>
+    <t>Zeeshan Siddiqi</t>
   </si>
   <si>
     <t>PC de Silva</t>
   </si>
   <si>
-    <t>Al-Amin Hossain</t>
-  </si>
-  <si>
-    <t>AM Phangiso</t>
-  </si>
-  <si>
-    <t>KV Jain</t>
+    <t>Mohammad Talha</t>
+  </si>
+  <si>
+    <t>LR Johnson</t>
+  </si>
+  <si>
+    <t>SS Cottrell</t>
   </si>
   <si>
     <t>VR Vanitha</t>
   </si>
   <si>
-    <t>KL Cross</t>
-  </si>
-  <si>
     <t>SA Abbott</t>
   </si>
   <si>
+    <t>Zulfiqar Babar</t>
+  </si>
+  <si>
     <t>Raza Hasan</t>
   </si>
   <si>
-    <t>Zulfiqar Babar</t>
-  </si>
-  <si>
     <t>J Anderson</t>
   </si>
   <si>
@@ -3556,13 +3907,13 @@
     <t>J Nyumbu</t>
   </si>
   <si>
-    <t>Irfan Ahmed</t>
-  </si>
-  <si>
-    <t>Skhawat Ali</t>
-  </si>
-  <si>
-    <t>JJ Atkinson</t>
+    <t>Salman Faris</t>
+  </si>
+  <si>
+    <t>Fayyaz Ahmed</t>
+  </si>
+  <si>
+    <t>Irfan Sajid</t>
   </si>
   <si>
     <t>Waqas Barkat</t>
@@ -3580,37 +3931,34 @@
     <t>JA Burns</t>
   </si>
   <si>
+    <t>AC Agar</t>
+  </si>
+  <si>
     <t>RJW Topley</t>
   </si>
   <si>
-    <t>CA Pujara</t>
+    <t>Mohammad Mithun</t>
   </si>
   <si>
     <t>Sania Khan</t>
   </si>
   <si>
-    <t>SL Quintyne</t>
-  </si>
-  <si>
     <t>Sharafuddin Ashraf</t>
   </si>
   <si>
-    <t>Aftab Alam</t>
-  </si>
-  <si>
     <t>APS Lakshika</t>
   </si>
   <si>
     <t>B Bezuidenhout</t>
   </si>
   <si>
-    <t>Y Fourie</t>
-  </si>
-  <si>
     <t>PLS Gamage</t>
   </si>
   <si>
-    <t>Sumaiya Siddiqi</t>
+    <t>RL Grundy</t>
+  </si>
+  <si>
+    <t>D Wiese</t>
   </si>
   <si>
     <t>Liton Das</t>
@@ -3619,7 +3967,7 @@
     <t>Jubair Hossain</t>
   </si>
   <si>
-    <t>D Wiese</t>
+    <t>NA Moodley</t>
   </si>
   <si>
     <t>Saad Nasim</t>
@@ -3628,21 +3976,9 @@
     <t>Sami Aslam</t>
   </si>
   <si>
-    <t>DS Kulkarni</t>
-  </si>
-  <si>
-    <t>ML Green</t>
-  </si>
-  <si>
-    <t>MJG Nielsen</t>
-  </si>
-  <si>
     <t>GA Guy</t>
   </si>
   <si>
-    <t>KE Broadmore</t>
-  </si>
-  <si>
     <t>Gurkeerat Singh</t>
   </si>
   <si>
@@ -3655,21 +3991,42 @@
     <t>Zafar Gohar</t>
   </si>
   <si>
+    <t>Asif Iqbal (1)</t>
+  </si>
+  <si>
+    <t>Umair Ali</t>
+  </si>
+  <si>
+    <t>L Sreekumar</t>
+  </si>
+  <si>
+    <t>Abdul Shakoor</t>
+  </si>
+  <si>
+    <t>Y Punja</t>
+  </si>
+  <si>
+    <t>Zaheer Maqsood</t>
+  </si>
+  <si>
     <t>MD Shanaka</t>
   </si>
   <si>
+    <t>KMC Bandara</t>
+  </si>
+  <si>
     <t>LA Dawson</t>
   </si>
   <si>
     <t>JDF Vandersay</t>
   </si>
   <si>
+    <t>SM Boland</t>
+  </si>
+  <si>
     <t>J Blackwood</t>
   </si>
   <si>
-    <t>NND de Silva</t>
-  </si>
-  <si>
     <t>TMM Newton</t>
   </si>
   <si>
@@ -3679,19 +4036,13 @@
     <t>Shamima Sultana</t>
   </si>
   <si>
-    <t>Nahida Akter</t>
-  </si>
-  <si>
-    <t>L Goodall</t>
-  </si>
-  <si>
     <t>SP Terry</t>
   </si>
   <si>
     <t>DJ Worrall</t>
   </si>
   <si>
-    <t>SM Boland</t>
+    <t>JM Mennie</t>
   </si>
   <si>
     <t>CP Tremain</t>
@@ -3700,60 +4051,33 @@
     <t>DS Weerakkody</t>
   </si>
   <si>
-    <t>CBRLS Kumara</t>
-  </si>
-  <si>
     <t>Sidra Ameen</t>
   </si>
   <si>
     <t>Yamin Ahmadzai</t>
   </si>
   <si>
+    <t>U Raymond-Hoey</t>
+  </si>
+  <si>
+    <t>CC Dalton</t>
+  </si>
+  <si>
     <t>MA Aponso</t>
   </si>
   <si>
     <t>WIA Fernando</t>
   </si>
   <si>
-    <t>AK Perera</t>
-  </si>
-  <si>
-    <t>L Sreekumar</t>
-  </si>
-  <si>
-    <t>Saqlain Haider</t>
-  </si>
-  <si>
-    <t>Fayyaz Ahmed</t>
-  </si>
-  <si>
-    <t>RAJ Smith</t>
-  </si>
-  <si>
     <t>BB Sran</t>
   </si>
   <si>
-    <t>Subashis Roy</t>
-  </si>
-  <si>
     <t>T Shamsi</t>
   </si>
   <si>
-    <t>Shadab Khan</t>
-  </si>
-  <si>
-    <t>Fahim Ashraf</t>
-  </si>
-  <si>
     <t>Rumman Raees</t>
   </si>
   <si>
-    <t>WT Gavera</t>
-  </si>
-  <si>
-    <t>K Christie</t>
-  </si>
-  <si>
     <t>KA Maharaj</t>
   </si>
   <si>
@@ -3763,31 +4087,7 @@
     <t>Sunzamul Islam</t>
   </si>
   <si>
-    <t>Simi Singh</t>
-  </si>
-  <si>
-    <t>J Mulder</t>
-  </si>
-  <si>
-    <t>A Bosch</t>
-  </si>
-  <si>
-    <t>Naveen-ul-Haq</t>
-  </si>
-  <si>
-    <t>WGAKK Kulasuriya</t>
-  </si>
-  <si>
-    <t>ML Cummins</t>
-  </si>
-  <si>
-    <t>M Shehani</t>
-  </si>
-  <si>
-    <t>LN McCarthy</t>
-  </si>
-  <si>
-    <t>RS Gayakwad</t>
+    <t>SK Yadav</t>
   </si>
   <si>
     <t>Qadeer Ahmed</t>
@@ -3796,16 +4096,13 @@
     <t>B Vakarewa</t>
   </si>
   <si>
-    <t>L Little</t>
-  </si>
-  <si>
     <t>S MacMahon</t>
   </si>
   <si>
-    <t>Kuldeep Yadav</t>
-  </si>
-  <si>
-    <t>GJP Kruger</t>
+    <t>AM Fernando</t>
+  </si>
+  <si>
+    <t>AGR Loudon</t>
   </si>
   <si>
     <t>M Zondeki</t>
@@ -3814,52 +4111,22 @@
     <t>Arshad Khan</t>
   </si>
   <si>
-    <t>ML Lewis</t>
-  </si>
-  <si>
     <t>Tapash Baisya</t>
   </si>
   <si>
-    <t>Manjural Islam Rana</t>
-  </si>
-  <si>
     <t>DJ Cullen</t>
   </si>
   <si>
-    <t>DK Butler</t>
-  </si>
-  <si>
     <t>MJ Hoggard</t>
   </si>
   <si>
-    <t>KT Sandher</t>
-  </si>
-  <si>
-    <t>S Thuraisingam</t>
-  </si>
-  <si>
-    <t>A Codrington</t>
-  </si>
-  <si>
-    <t>RR Emrit</t>
-  </si>
-  <si>
     <t>AA Noffke</t>
   </si>
   <si>
-    <t>IE O'Brien</t>
-  </si>
-  <si>
-    <t>AS Luseno</t>
-  </si>
-  <si>
     <t>PL Harris</t>
   </si>
   <si>
-    <t>Sami Faridi</t>
-  </si>
-  <si>
-    <t>PC Connell</t>
+    <t>TE Tucker</t>
   </si>
   <si>
     <t>Samiullah Khan</t>
@@ -3868,76 +4135,25 @@
     <t>Rizwan Ahmed</t>
   </si>
   <si>
-    <t>Zahid Shah</t>
-  </si>
-  <si>
-    <t>Fahad Alhashmi</t>
-  </si>
-  <si>
-    <t>EHSN Silva</t>
-  </si>
-  <si>
-    <t>Saqib Ali</t>
-  </si>
-  <si>
-    <t>Arshad Ali</t>
-  </si>
-  <si>
-    <t>Afzaal Haider</t>
-  </si>
-  <si>
-    <t>Zain Abbas</t>
-  </si>
-  <si>
-    <t>Najeeb Amar</t>
-  </si>
-  <si>
-    <t>Munir Dar</t>
-  </si>
-  <si>
-    <t>JPR Lamsam</t>
-  </si>
-  <si>
-    <t>Aman Ali</t>
-  </si>
-  <si>
     <t>MS Gony</t>
   </si>
   <si>
-    <t>Mansoor Amjad</t>
-  </si>
-  <si>
-    <t>B Geeves</t>
-  </si>
-  <si>
-    <t>SM Harwood</t>
-  </si>
-  <si>
-    <t>BJ Diamanti</t>
-  </si>
-  <si>
     <t>IT Guha</t>
   </si>
   <si>
     <t>NJ Shaw</t>
   </si>
   <si>
-    <t>Mahbubul Alam</t>
-  </si>
-  <si>
-    <t>RM West</t>
+    <t>EP Thompson</t>
   </si>
   <si>
     <t>BL Morgan</t>
   </si>
   <si>
-    <t>L Balaji</t>
-  </si>
-  <si>
-    <t>NT Pascal</t>
-  </si>
-  <si>
-    <t>AM Nayar</t>
+    <t>E Katchay</t>
+  </si>
+  <si>
+    <t>Dawlat Ahmadzai</t>
   </si>
   <si>
     <t>C van der Westhuizen</t>
@@ -3946,115 +4162,55 @@
     <t>AE Smith</t>
   </si>
   <si>
-    <t>S Tyagi</t>
-  </si>
-  <si>
-    <t>BA Westdijk</t>
-  </si>
-  <si>
-    <t>TG Gordon</t>
-  </si>
-  <si>
-    <t>A Mithun</t>
-  </si>
-  <si>
-    <t>IA Nicolson</t>
-  </si>
-  <si>
     <t>G Goudie</t>
   </si>
   <si>
-    <t>R Sharma</t>
-  </si>
-  <si>
-    <t>VR Aaron</t>
-  </si>
-  <si>
-    <t>Zahid Hussain</t>
-  </si>
-  <si>
     <t>GW Aldridge</t>
   </si>
   <si>
     <t>N Ncube</t>
   </si>
   <si>
-    <t>K Thomson</t>
-  </si>
-  <si>
     <t>DR Briggs</t>
   </si>
   <si>
-    <t>Elias Sunny</t>
-  </si>
-  <si>
-    <t>DI Allan</t>
+    <t>S Weerakoon</t>
   </si>
   <si>
     <t>I Udana</t>
   </si>
   <si>
-    <t>SEA Ruck</t>
-  </si>
-  <si>
-    <t>RH Candy</t>
-  </si>
-  <si>
     <t>NM Odhiambo</t>
   </si>
   <si>
+    <t>N Dutta</t>
+  </si>
+  <si>
+    <t>RK Parwin</t>
+  </si>
+  <si>
     <t>S Ravikumar</t>
   </si>
   <si>
-    <t>S Sharma</t>
-  </si>
-  <si>
-    <t>LHD Dilhara</t>
-  </si>
-  <si>
-    <t>NM Carter</t>
-  </si>
-  <si>
     <t>SL Munroe</t>
   </si>
   <si>
     <t>JD Unadkat</t>
   </si>
   <si>
-    <t>MEMO Scott-Hayward</t>
-  </si>
-  <si>
-    <t>EJ Tice</t>
-  </si>
-  <si>
-    <t>EAJ Richardson</t>
-  </si>
-  <si>
-    <t>Kamran Shazad</t>
-  </si>
-  <si>
-    <t>EJ Richardson</t>
-  </si>
-  <si>
     <t>Y Potgieter</t>
   </si>
   <si>
+    <t>PA van Meekeren</t>
+  </si>
+  <si>
     <t>VJ Kingma</t>
   </si>
   <si>
-    <t>Mohammad Talha</t>
-  </si>
-  <si>
-    <t>SS Cottrell</t>
-  </si>
-  <si>
     <t>M Shezi</t>
   </si>
   <si>
-    <t>Irfan Sajid</t>
-  </si>
-  <si>
-    <t>AC Agar</t>
+    <t>AW Mathieson</t>
   </si>
   <si>
     <t>Parvez Rasool</t>
@@ -4066,9 +4222,6 @@
     <t>KV Sharma</t>
   </si>
   <si>
-    <t>RL Grundy</t>
-  </si>
-  <si>
     <t>Salman Farooq</t>
   </si>
   <si>
@@ -4076,24 +4229,6 @@
   </si>
   <si>
     <t>JS Paris</t>
-  </si>
-  <si>
-    <t>Y Punja</t>
-  </si>
-  <si>
-    <t>Umair Ali</t>
-  </si>
-  <si>
-    <t>Zaheer Maqsood</t>
-  </si>
-  <si>
-    <t>Asif Iqbal (1)</t>
-  </si>
-  <si>
-    <t>KMC Bandara</t>
-  </si>
-  <si>
-    <t>JM Mennie</t>
   </si>
   <si>
     <t>Rokhan Barakzai</t>
@@ -4466,7 +4601,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1362"/>
+  <dimension ref="A1:B1407"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4474,7 +4609,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>1361</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -15363,6 +15498,366 @@
       </c>
       <c r="B1362" t="s">
         <v>1360</v>
+      </c>
+    </row>
+    <row r="1363" spans="1:2">
+      <c r="A1363" s="2">
+        <v>1361</v>
+      </c>
+      <c r="B1363" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="1364" spans="1:2">
+      <c r="A1364" s="2">
+        <v>1362</v>
+      </c>
+      <c r="B1364" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="1365" spans="1:2">
+      <c r="A1365" s="2">
+        <v>1363</v>
+      </c>
+      <c r="B1365" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="1366" spans="1:2">
+      <c r="A1366" s="2">
+        <v>1364</v>
+      </c>
+      <c r="B1366" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="1367" spans="1:2">
+      <c r="A1367" s="2">
+        <v>1365</v>
+      </c>
+      <c r="B1367" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="1368" spans="1:2">
+      <c r="A1368" s="2">
+        <v>1366</v>
+      </c>
+      <c r="B1368" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="1369" spans="1:2">
+      <c r="A1369" s="2">
+        <v>1367</v>
+      </c>
+      <c r="B1369" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="1370" spans="1:2">
+      <c r="A1370" s="2">
+        <v>1368</v>
+      </c>
+      <c r="B1370" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="1371" spans="1:2">
+      <c r="A1371" s="2">
+        <v>1369</v>
+      </c>
+      <c r="B1371" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="1372" spans="1:2">
+      <c r="A1372" s="2">
+        <v>1370</v>
+      </c>
+      <c r="B1372" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="1373" spans="1:2">
+      <c r="A1373" s="2">
+        <v>1371</v>
+      </c>
+      <c r="B1373" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="1374" spans="1:2">
+      <c r="A1374" s="2">
+        <v>1372</v>
+      </c>
+      <c r="B1374" t="s">
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="1375" spans="1:2">
+      <c r="A1375" s="2">
+        <v>1373</v>
+      </c>
+      <c r="B1375" t="s">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="1376" spans="1:2">
+      <c r="A1376" s="2">
+        <v>1374</v>
+      </c>
+      <c r="B1376" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="1377" spans="1:2">
+      <c r="A1377" s="2">
+        <v>1375</v>
+      </c>
+      <c r="B1377" t="s">
+        <v>1375</v>
+      </c>
+    </row>
+    <row r="1378" spans="1:2">
+      <c r="A1378" s="2">
+        <v>1376</v>
+      </c>
+      <c r="B1378" t="s">
+        <v>1376</v>
+      </c>
+    </row>
+    <row r="1379" spans="1:2">
+      <c r="A1379" s="2">
+        <v>1377</v>
+      </c>
+      <c r="B1379" t="s">
+        <v>1377</v>
+      </c>
+    </row>
+    <row r="1380" spans="1:2">
+      <c r="A1380" s="2">
+        <v>1378</v>
+      </c>
+      <c r="B1380" t="s">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="1381" spans="1:2">
+      <c r="A1381" s="2">
+        <v>1379</v>
+      </c>
+      <c r="B1381" t="s">
+        <v>1379</v>
+      </c>
+    </row>
+    <row r="1382" spans="1:2">
+      <c r="A1382" s="2">
+        <v>1380</v>
+      </c>
+      <c r="B1382" t="s">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="1383" spans="1:2">
+      <c r="A1383" s="2">
+        <v>1381</v>
+      </c>
+      <c r="B1383" t="s">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="1384" spans="1:2">
+      <c r="A1384" s="2">
+        <v>1382</v>
+      </c>
+      <c r="B1384" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="1385" spans="1:2">
+      <c r="A1385" s="2">
+        <v>1383</v>
+      </c>
+      <c r="B1385" t="s">
+        <v>1383</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:2">
+      <c r="A1386" s="2">
+        <v>1384</v>
+      </c>
+      <c r="B1386" t="s">
+        <v>1384</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:2">
+      <c r="A1387" s="2">
+        <v>1385</v>
+      </c>
+      <c r="B1387" t="s">
+        <v>1385</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:2">
+      <c r="A1388" s="2">
+        <v>1386</v>
+      </c>
+      <c r="B1388" t="s">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:2">
+      <c r="A1389" s="2">
+        <v>1387</v>
+      </c>
+      <c r="B1389" t="s">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:2">
+      <c r="A1390" s="2">
+        <v>1388</v>
+      </c>
+      <c r="B1390" t="s">
+        <v>1388</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:2">
+      <c r="A1391" s="2">
+        <v>1389</v>
+      </c>
+      <c r="B1391" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:2">
+      <c r="A1392" s="2">
+        <v>1390</v>
+      </c>
+      <c r="B1392" t="s">
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:2">
+      <c r="A1393" s="2">
+        <v>1391</v>
+      </c>
+      <c r="B1393" t="s">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:2">
+      <c r="A1394" s="2">
+        <v>1392</v>
+      </c>
+      <c r="B1394" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:2">
+      <c r="A1395" s="2">
+        <v>1393</v>
+      </c>
+      <c r="B1395" t="s">
+        <v>1393</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:2">
+      <c r="A1396" s="2">
+        <v>1394</v>
+      </c>
+      <c r="B1396" t="s">
+        <v>1394</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:2">
+      <c r="A1397" s="2">
+        <v>1395</v>
+      </c>
+      <c r="B1397" t="s">
+        <v>1395</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:2">
+      <c r="A1398" s="2">
+        <v>1396</v>
+      </c>
+      <c r="B1398" t="s">
+        <v>1396</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:2">
+      <c r="A1399" s="2">
+        <v>1397</v>
+      </c>
+      <c r="B1399" t="s">
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:2">
+      <c r="A1400" s="2">
+        <v>1398</v>
+      </c>
+      <c r="B1400" t="s">
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:2">
+      <c r="A1401" s="2">
+        <v>1399</v>
+      </c>
+      <c r="B1401" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:2">
+      <c r="A1402" s="2">
+        <v>1400</v>
+      </c>
+      <c r="B1402" t="s">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:2">
+      <c r="A1403" s="2">
+        <v>1401</v>
+      </c>
+      <c r="B1403" t="s">
+        <v>1401</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:2">
+      <c r="A1404" s="2">
+        <v>1402</v>
+      </c>
+      <c r="B1404" t="s">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:2">
+      <c r="A1405" s="2">
+        <v>1403</v>
+      </c>
+      <c r="B1405" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:2">
+      <c r="A1406" s="2">
+        <v>1404</v>
+      </c>
+      <c r="B1406" t="s">
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:2">
+      <c r="A1407" s="2">
+        <v>1405</v>
+      </c>
+      <c r="B1407" t="s">
+        <v>1405</v>
       </c>
     </row>
   </sheetData>

</xml_diff>